<commit_message>
updated an entry in the excel file
</commit_message>
<xml_diff>
--- a/address_file.xlsx
+++ b/address_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ameer.Shaik\Downloads\dsa\companies\props_amc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ameer.Shaik\Downloads\dsa\companies\props_amc\real_estate_suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C707BF1F-9F34-4047-A07B-B1E378990624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281E6D6A-F589-4115-9D13-F5431E6812DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3132" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="custom_sheet_name" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Address</t>
   </si>
   <si>
     <t>1600 Amphitheatre Parkway, Mountain View, CA</t>
-  </si>
-  <si>
-    <t>Unique Concord, Tata Nagar, Bangalore</t>
   </si>
   <si>
     <t>Mountain View, CA</t>
@@ -363,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,11 +391,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>